<commit_message>
update Shift Unit design
</commit_message>
<xml_diff>
--- a/pt1/ExU/Documentation/pt2/FP-log-G18-5593-350-1201.xlsx
+++ b/pt1/ExU/Documentation/pt2/FP-log-G18-5593-350-1201.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izyl\Desktop\shit1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izyl\Desktop\ensc350-final-project\pt1\ExU\Documentation\pt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9268C8DC-43CA-48A9-8D25-32AB9478B88C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0595C838-55A1-499B-9672-3975D39E6F9B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -131,6 +131,27 @@
   </si>
   <si>
     <t>Organizing file structure and pushed to repo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designed Execution Unit </t>
+  </si>
+  <si>
+    <t>Designed Shift Unit</t>
+  </si>
+  <si>
+    <t>Debug Shift Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug Execution Unit </t>
+  </si>
+  <si>
+    <t>Created circuit diagrams for Shift Unit and Execution Unit</t>
+  </si>
+  <si>
+    <t>Shift Unit Documentation (Sections: Functional Behaviour, VHDL Interface)</t>
+  </si>
+  <si>
+    <t>Updating design of Shift Unit</t>
   </si>
 </sst>
 </file>
@@ -2692,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD091BD6-3364-44DE-8BB4-985458F62AD8}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2802,92 +2823,148 @@
     <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="33"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="23"/>
+      <c r="C7" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E7" s="23">
+        <v>1</v>
+      </c>
       <c r="F7" s="34"/>
-      <c r="G7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="H7" s="27">
         <f>(E7-D7)*24</f>
-        <v>0</v>
+        <v>3.9999999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="33"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="23"/>
+      <c r="C8" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.5</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
-        <v>0</v>
+        <v>1.9999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="33"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23"/>
+      <c r="C9" s="22">
+        <v>43932</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="H9" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="33"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="23"/>
+      <c r="C10" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.375</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="F10" s="34"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="H10" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9999999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="33"/>
       <c r="B11" s="14"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="23"/>
+      <c r="C11" s="22">
+        <v>43933</v>
+      </c>
+      <c r="D11" s="20">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="H11" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9999999999999982</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="33"/>
       <c r="B12" s="14"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="22">
+        <v>43934</v>
+      </c>
+      <c r="D12" s="20">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="F12" s="34"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="H12" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="33"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="23"/>
+      <c r="C13" s="22">
+        <v>43935</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.75</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>23</v>
+      </c>
       <c r="H13" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.0000000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3739,7 +3816,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>1.9999999999999982</v>
+        <v>18.499999999999993</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>